<commit_message>
change the DH parameter
</commit_message>
<xml_diff>
--- a/Ginger DH Parameter.xlsx
+++ b/Ginger DH Parameter.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="192">
   <si>
     <t xml:space="preserve">Ginger DH Parameter</t>
   </si>
@@ -244,6 +244,7 @@
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">S</t>
     </r>
@@ -254,6 +255,7 @@
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -263,6 +265,7 @@
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-1.92</t>
     </r>
@@ -273,6 +276,7 @@
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -485,7 +489,7 @@
     <t xml:space="preserve">Right_Shoulder_X(2)</t>
   </si>
   <si>
-    <t xml:space="preserve">注：1和2之间的坐标系不是严格按照DH规则建立，因此单独计算1和2之间的旋转矩阵</t>
+    <t xml:space="preserve">注：1和2之间的坐标系不是严格按照DH规则建立，因此单独计算1和2之间的固定旋转矩阵</t>
   </si>
   <si>
     <t xml:space="preserve">Right_Shoulder_Y(3)</t>
@@ -497,10 +501,51 @@
     <t xml:space="preserve">Right_Elbow_X(5)</t>
   </si>
   <si>
-    <t xml:space="preserve">B*sθ(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A=0.3420201433</t>
+    <t xml:space="preserve">C(-1.22)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-S</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-1.22</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Right Shoulder</t>
@@ -509,25 +554,13 @@
     <t xml:space="preserve">Right_Wrist_Z(6)</t>
   </si>
   <si>
-    <t xml:space="preserve">C*cθ(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D*sθ(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B=-0.3420201433</t>
+    <t xml:space="preserve">S(-1.22)</t>
   </si>
   <si>
     <t xml:space="preserve">Right_Wrist_X(7)</t>
   </si>
   <si>
-    <t xml:space="preserve">C=-0.93969262</t>
-  </si>
-  <si>
     <t xml:space="preserve">Right_Wrist_Y(8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D=0.93969262</t>
   </si>
   <si>
     <t xml:space="preserve">Right_Wrist_Y(1)</t>
@@ -654,7 +687,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -700,17 +733,12 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -804,7 +832,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -835,8 +863,8 @@
   </sheetPr>
   <dimension ref="A1:AA102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q24" activeCellId="0" sqref="Q24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q68" activeCellId="0" sqref="Q68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -846,14 +874,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="8.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="8.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="13" style="1" width="8.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="13" style="1" width="8.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="8.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="19" style="1" width="8.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="19" style="1" width="8.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="8.63"/>
   </cols>
   <sheetData>
@@ -2948,7 +2976,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="3" t="s">
         <v>145</v>
       </c>
@@ -2971,22 +2999,19 @@
         <v>74</v>
       </c>
       <c r="M65" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N65" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="O65" s="7" t="n">
-        <v>-0.93969262</v>
+      <c r="N65" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O65" s="12" t="s">
+        <v>147</v>
       </c>
       <c r="P65" s="7" t="n">
-        <v>0.1634</v>
-      </c>
-      <c r="R65" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-0.1634</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="10" t="s">
         <v>148</v>
       </c>
@@ -3015,25 +3040,22 @@
       <c r="L66" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="M66" s="7" t="s">
+      <c r="M66" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="N66" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="O66" s="7" t="n">
-        <v>-0.3420201433</v>
+      <c r="N66" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" s="12" t="s">
+        <v>146</v>
       </c>
       <c r="P66" s="7" t="n">
         <v>-0.2581</v>
       </c>
-      <c r="R66" s="0" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D67" s="1" t="n">
         <v>0</v>
@@ -3053,11 +3075,11 @@
       <c r="I67" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M67" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="N67" s="7" t="s">
-        <v>41</v>
+      <c r="M67" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N67" s="7" t="n">
+        <v>-1</v>
       </c>
       <c r="O67" s="7" t="n">
         <v>0</v>
@@ -3065,13 +3087,10 @@
       <c r="P67" s="7" t="n">
         <v>0.017</v>
       </c>
-      <c r="R67" s="0" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D68" s="1" t="n">
         <v>0</v>
@@ -3103,9 +3122,6 @@
       <c r="P68" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="R68" s="0" t="s">
-        <v>156</v>
-      </c>
     </row>
     <row r="69" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="13"/>
@@ -3115,7 +3131,7 @@
     </row>
     <row r="71" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>11</v>
@@ -3154,7 +3170,7 @@
       </c>
       <c r="B72" s="10"/>
       <c r="C72" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>91</v>
@@ -3165,10 +3181,10 @@
         <v>18</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="L72" s="0" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="M72" s="1" t="s">
         <v>106</v>
@@ -3183,7 +3199,7 @@
         <v>-0.0941606527701362</v>
       </c>
       <c r="R72" s="0" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="S72" s="1" t="s">
         <v>28</v>
@@ -3200,13 +3216,13 @@
     </row>
     <row r="73" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="M73" s="1" t="n">
         <v>0</v>
@@ -3235,13 +3251,13 @@
     </row>
     <row r="74" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>33</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="M74" s="1" t="n">
         <v>0</v>
@@ -3276,7 +3292,7 @@
     </row>
     <row r="77" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>11</v>
@@ -3330,7 +3346,7 @@
       </c>
       <c r="B78" s="10"/>
       <c r="C78" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>18</v>
@@ -3339,10 +3355,10 @@
         <v>0</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L78" s="13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="M78" s="1" t="s">
         <v>106</v>
@@ -3357,7 +3373,7 @@
         <v>-0.116385781256913</v>
       </c>
       <c r="Q78" s="13" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="R78" s="1" t="s">
         <v>28</v>
@@ -3372,7 +3388,7 @@
         <v>-0.025999999071151</v>
       </c>
       <c r="V78" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="W78" s="1" t="s">
         <v>55</v>
@@ -3389,7 +3405,7 @@
     </row>
     <row r="79" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>110</v>
@@ -3403,7 +3419,7 @@
         <v>0</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="M79" s="1" t="n">
         <v>0</v>
@@ -3444,7 +3460,7 @@
     </row>
     <row r="80" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>33</v>
@@ -3453,7 +3469,7 @@
         <v>0</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="M80" s="1" t="n">
         <v>0</v>
@@ -3494,7 +3510,7 @@
     </row>
     <row r="81" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>36</v>
@@ -3503,7 +3519,7 @@
         <v>0</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3514,7 +3530,7 @@
     </row>
     <row r="84" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>11</v>
@@ -3568,7 +3584,7 @@
       </c>
       <c r="B85" s="10"/>
       <c r="C85" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>18</v>
@@ -3577,10 +3593,10 @@
         <v>0</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="L85" s="13" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="M85" s="1" t="s">
         <v>106</v>
@@ -3595,7 +3611,7 @@
         <v>-0.121385781256913</v>
       </c>
       <c r="Q85" s="13" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="R85" s="1" t="s">
         <v>28</v>
@@ -3610,7 +3626,7 @@
         <v>-0.0259999990711514</v>
       </c>
       <c r="V85" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="W85" s="1" t="s">
         <v>55</v>
@@ -3627,7 +3643,7 @@
     </row>
     <row r="86" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>110</v>
@@ -3641,7 +3657,7 @@
         <v>0</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M86" s="1" t="n">
         <v>0</v>
@@ -3682,7 +3698,7 @@
     </row>
     <row r="87" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>33</v>
@@ -3691,7 +3707,7 @@
         <v>0</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M87" s="1" t="n">
         <v>0</v>
@@ -3732,7 +3748,7 @@
     </row>
     <row r="88" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>36</v>
@@ -3741,7 +3757,7 @@
         <v>0</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3752,7 +3768,7 @@
     </row>
     <row r="91" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>11</v>
@@ -3806,7 +3822,7 @@
       </c>
       <c r="B92" s="10"/>
       <c r="C92" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>18</v>
@@ -3815,10 +3831,10 @@
         <v>0</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="L92" s="13" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="M92" s="1" t="s">
         <v>106</v>
@@ -3833,7 +3849,7 @@
         <v>-0.113385771822664</v>
       </c>
       <c r="Q92" s="13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="R92" s="1" t="s">
         <v>28</v>
@@ -3848,7 +3864,7 @@
         <v>-0.0260000085054002</v>
       </c>
       <c r="V92" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="W92" s="1" t="s">
         <v>55</v>
@@ -3865,7 +3881,7 @@
     </row>
     <row r="93" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>110</v>
@@ -3879,7 +3895,7 @@
         <v>0</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="M93" s="1" t="n">
         <v>0</v>
@@ -3920,7 +3936,7 @@
     </row>
     <row r="94" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>33</v>
@@ -3929,7 +3945,7 @@
         <v>0</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="M94" s="1" t="n">
         <v>0</v>
@@ -3970,7 +3986,7 @@
     </row>
     <row r="95" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>36</v>
@@ -3979,7 +3995,7 @@
         <v>0</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3990,7 +4006,7 @@
     </row>
     <row r="98" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>11</v>
@@ -4044,7 +4060,7 @@
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>18</v>
@@ -4053,10 +4069,10 @@
         <v>0</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="L99" s="13" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="M99" s="1" t="s">
         <v>106</v>
@@ -4071,7 +4087,7 @@
         <v>-0.108682998728874</v>
       </c>
       <c r="Q99" s="13" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="R99" s="1" t="s">
         <v>28</v>
@@ -4086,7 +4102,7 @@
         <v>-0.023451660741343</v>
       </c>
       <c r="V99" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="W99" s="1" t="s">
         <v>55</v>
@@ -4103,7 +4119,7 @@
     </row>
     <row r="100" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>110</v>
@@ -4117,7 +4133,7 @@
         <v>0</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="M100" s="1" t="n">
         <v>0</v>
@@ -4158,7 +4174,7 @@
     </row>
     <row r="101" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>33</v>
@@ -4167,7 +4183,7 @@
         <v>0</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="M101" s="1" t="n">
         <v>0</v>
@@ -4208,7 +4224,7 @@
     </row>
     <row r="102" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>36</v>
@@ -4217,7 +4233,7 @@
         <v>0</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>